<commit_message>
updated the excel reformatting and dynamic recipient
</commit_message>
<xml_diff>
--- a/testData/MMT_Test_Data.xlsx
+++ b/testData/MMT_Test_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2355257\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2355257\Desktop\LEARN_AUTOMATION\automation\HACKATHON_TEAM\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{624935CD-20B2-41C9-94FA-1B9733CFA9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D5CA54D-85CF-4C95-ADD9-28E2A6F7F0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7993C069-6278-478B-9354-E911B3E7BF11}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>From</t>
   </si>
@@ -91,16 +91,33 @@
   </si>
   <si>
     <t>sssdd</t>
+  </si>
+  <si>
+    <t>9900443322</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,14 +140,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,7 +487,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,10 +548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DF4F46-836E-4410-AAFF-F750383D5046}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,7 +562,7 @@
     <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -554,22 +575,32 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>5000</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>2000</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1">
-        <v>9900443322</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="sssdd@gmail.com" xr:uid="{8A125A72-214F-4C93-BA4A-6F66F06228B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>